<commit_message>
Removing explicit emission penalty
Only use CO2 price (more intuitive)
</commit_message>
<xml_diff>
--- a/Data/transport_costs_emissions.xlsx
+++ b/Data/transport_costs_emissions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_37D19DEF87815E2EFBD92C11595ED87656C9AF45" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD742ABC-9DAC-407F-B615-E979A66E57B8}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_37D19DEF87815E2EFBD92C11595ED87656C9AF45" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9363B5D6-4875-416F-A11A-857B7E2F9942}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="0" windowWidth="30345" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,7 +304,17 @@
   <autoFilter ref="A1:H631" xr:uid="{74AC4D21-4694-4090-9C4D-A67DC2D32754}">
     <filterColumn colId="4">
       <filters>
-        <filter val="Hydrogen"/>
+        <filter val="Biodiesel"/>
+        <filter val="Biogas"/>
+        <filter val="Diesel"/>
+        <filter val="HFO"/>
+        <filter val="LNG"/>
+        <filter val="MGO"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="2022"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -610,7 +620,7 @@
   <dimension ref="A1:H631"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+      <selection activeCell="H2" sqref="H2:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -700,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -726,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -752,7 +762,7 @@
         <v>9.3478260869565233</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -778,7 +788,7 @@
         <v>8.4782608695652186</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -830,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -856,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -882,7 +892,7 @@
         <v>5.2121212121212119</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -908,7 +918,7 @@
         <v>4.7272727272727284</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -960,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -986,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1012,7 +1022,7 @@
         <v>5.2121212121212119</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1038,7 +1048,7 @@
         <v>4.7272727272727284</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1090,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1116,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1142,7 +1152,7 @@
         <v>5.2121212121212119</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1168,7 +1178,7 @@
         <v>4.7272727272727284</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1220,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1246,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1272,7 +1282,7 @@
         <v>5.2121212121212119</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1298,7 +1308,7 @@
         <v>4.7272727272727284</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1350,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1402,7 +1412,7 @@
         <v>5.0588235294117636</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1428,7 +1438,7 @@
         <v>4.5882352941176467</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1480,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1506,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1532,7 +1542,7 @@
         <v>5.2121212121212119</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1558,7 +1568,7 @@
         <v>4.7272727272727284</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1584,7 +1594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1610,7 +1620,7 @@
         <v>12.09</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1636,7 +1646,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1714,7 +1724,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1740,7 +1750,7 @@
         <v>3.12</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1766,7 +1776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1792,7 +1802,7 @@
         <v>25.11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1818,7 +1828,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1896,7 +1906,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1922,7 +1932,7 @@
         <v>6.48</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1948,7 +1958,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1974,7 +1984,7 @@
         <v>25.11</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2000,7 +2010,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2078,7 +2088,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2104,7 +2114,7 @@
         <v>6.48</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2130,7 +2140,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2156,7 +2166,7 @@
         <v>25.11</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2182,7 +2192,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2260,7 +2270,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2286,7 +2296,7 @@
         <v>6.48</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2312,7 +2322,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2338,7 +2348,7 @@
         <v>16.274999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2364,7 +2374,7 @@
         <v>12.25</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2442,7 +2452,7 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2468,7 +2478,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2494,7 +2504,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2520,7 +2530,7 @@
         <v>16.274999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2546,7 +2556,7 @@
         <v>12.25</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2624,7 +2634,7 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2650,7 +2660,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2676,7 +2686,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2702,7 +2712,7 @@
         <v>12.648</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2728,7 +2738,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2806,7 +2816,7 @@
         <v>12.24</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2832,7 +2842,7 @@
         <v>3.2639999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2936,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2962,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2988,7 +2998,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3092,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3118,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3144,7 +3154,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3248,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3274,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3300,7 +3310,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3404,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3430,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3456,7 +3466,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3560,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3586,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3612,7 +3622,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3716,7 +3726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3742,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3768,7 +3778,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3872,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3898,7 +3908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3976,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -4106,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -4236,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4366,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -4496,7 +4506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -4626,7 +4636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -4756,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -4912,7 +4922,7 @@
         <v>8.8478629366490988</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -5094,7 +5104,7 @@
         <v>18.376330714578899</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -5276,7 +5286,7 @@
         <v>18.376330714578899</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -5458,7 +5468,7 @@
         <v>18.376330714578899</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -5640,7 +5650,7 @@
         <v>11.910584722412249</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -5822,7 +5832,7 @@
         <v>11.910584722412249</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -6004,7 +6014,7 @@
         <v>9.2562258414175211</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -6212,7 +6222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -6368,7 +6378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -6524,7 +6534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -6680,7 +6690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -6836,7 +6846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -6992,7 +7002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -7148,7 +7158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -7252,7 +7262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -7382,7 +7392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -7512,7 +7522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -7642,7 +7652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -7772,7 +7782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -7902,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -8032,7 +8042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -8188,7 +8198,7 @@
         <v>8.6027119281020674</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -8370,7 +8380,7 @@
         <v>17.8671709275966</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -8552,7 +8562,7 @@
         <v>17.8671709275966</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -8734,7 +8744,7 @@
         <v>17.8671709275966</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -8916,7 +8926,7 @@
         <v>11.58057374936817</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -9098,7 +9108,7 @@
         <v>11.58057374936817</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>325</v>
       </c>
@@ -9280,7 +9290,7 @@
         <v>8.9997601709375488</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -9488,7 +9498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -9644,7 +9654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -9800,7 +9810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -9956,7 +9966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>358</v>
       </c>
@@ -10112,7 +10122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -10268,7 +10278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>370</v>
       </c>
@@ -10424,7 +10434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>376</v>
       </c>
@@ -10528,7 +10538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>380</v>
       </c>
@@ -10658,7 +10668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>385</v>
       </c>
@@ -10788,7 +10798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>390</v>
       </c>
@@ -10918,7 +10928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>395</v>
       </c>
@@ -11048,7 +11058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>400</v>
       </c>
@@ -11178,7 +11188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>405</v>
       </c>
@@ -11308,7 +11318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>410</v>
       </c>
@@ -11464,7 +11474,7 @@
         <v>8.0191412866628866</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>416</v>
       </c>
@@ -11646,7 +11656,7 @@
         <v>16.65513959537676</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>423</v>
       </c>
@@ -11828,7 +11838,7 @@
         <v>16.65513959537676</v>
       </c>
     </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
         <v>430</v>
       </c>
@@ -12010,7 +12020,7 @@
         <v>16.65513959537676</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>437</v>
       </c>
@@ -12192,7 +12202,7 @@
         <v>10.79499788589235</v>
       </c>
     </row>
-    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
         <v>444</v>
       </c>
@@ -12374,7 +12384,7 @@
         <v>10.79499788589235</v>
       </c>
     </row>
-    <row r="453" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
         <v>451</v>
       </c>
@@ -12556,7 +12566,7 @@
         <v>8.3892554998934816</v>
       </c>
     </row>
-    <row r="460" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
         <v>458</v>
       </c>
@@ -12764,7 +12774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" s="1">
         <v>466</v>
       </c>
@@ -12920,7 +12930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="474" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" s="1">
         <v>472</v>
       </c>
@@ -13076,7 +13086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="480" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" s="1">
         <v>478</v>
       </c>
@@ -13232,7 +13242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" s="1">
         <v>484</v>
       </c>
@@ -13388,7 +13398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="492" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" s="1">
         <v>490</v>
       </c>
@@ -13544,7 +13554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="498" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" s="1">
         <v>496</v>
       </c>
@@ -13700,7 +13710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="504" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" s="1">
         <v>502</v>
       </c>
@@ -13804,7 +13814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="508" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" s="1">
         <v>506</v>
       </c>
@@ -13934,7 +13944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="513" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513" s="1">
         <v>511</v>
       </c>
@@ -14064,7 +14074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="518" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518" s="1">
         <v>516</v>
       </c>
@@ -14194,7 +14204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="523" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A523" s="1">
         <v>521</v>
       </c>
@@ -14324,7 +14334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="528" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A528" s="1">
         <v>526</v>
       </c>
@@ -14454,7 +14464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="533" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533" s="1">
         <v>531</v>
       </c>
@@ -14584,7 +14594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="538" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A538" s="1">
         <v>536</v>
       </c>
@@ -14740,7 +14750,7 @@
         <v>7.4751575448427943</v>
       </c>
     </row>
-    <row r="544" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A544" s="1">
         <v>542</v>
       </c>
@@ -14922,7 +14932,7 @@
         <v>15.52532720851965</v>
       </c>
     </row>
-    <row r="551" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A551" s="1">
         <v>549</v>
       </c>
@@ -15104,7 +15114,7 @@
         <v>15.52532720851965</v>
       </c>
     </row>
-    <row r="558" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A558" s="1">
         <v>556</v>
       </c>
@@ -15286,7 +15296,7 @@
         <v>15.52532720851965</v>
       </c>
     </row>
-    <row r="565" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A565" s="1">
         <v>563</v>
       </c>
@@ -15468,7 +15478,7 @@
         <v>10.06271207959607</v>
       </c>
     </row>
-    <row r="572" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A572" s="1">
         <v>570</v>
       </c>
@@ -15650,7 +15660,7 @@
         <v>10.06271207959607</v>
       </c>
     </row>
-    <row r="579" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A579" s="1">
         <v>577</v>
       </c>
@@ -15832,7 +15842,7 @@
         <v>7.8201648161432313</v>
       </c>
     </row>
-    <row r="586" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A586" s="1">
         <v>584</v>
       </c>
@@ -16040,7 +16050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="594" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A594" s="1">
         <v>592</v>
       </c>
@@ -16196,7 +16206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="600" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A600" s="1">
         <v>598</v>
       </c>
@@ -16352,7 +16362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="606" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A606" s="1">
         <v>604</v>
       </c>
@@ -16508,7 +16518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="612" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A612" s="1">
         <v>610</v>
       </c>
@@ -16664,7 +16674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="618" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A618" s="1">
         <v>616</v>
       </c>
@@ -16820,7 +16830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="624" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A624" s="1">
         <v>622</v>
       </c>
@@ -16976,7 +16986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="630" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="630" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A630" s="1">
         <v>628</v>
       </c>

</xml_diff>